<commit_message>
Updates to task breakdown
</commit_message>
<xml_diff>
--- a/DM2124/Task Breakdown.xlsx
+++ b/DM2124/Task Breakdown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sri\Desktop\School Repository\DM2124\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sri\Desktop\School-Stuff\DM2124\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,43 +24,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Progammer 1</t>
-  </si>
-  <si>
-    <t>Progammer 2</t>
-  </si>
-  <si>
-    <t>Artist 1</t>
-  </si>
-  <si>
-    <t>Artist 2</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>Create Concept Art for cosmetics</t>
-  </si>
-  <si>
-    <t>Create Concept Art for assets used in battles</t>
-  </si>
-  <si>
-    <t>Establish tasks to be done</t>
-  </si>
-  <si>
-    <t>Create Play board</t>
-  </si>
-  <si>
-    <t>Create match 3 basic functions</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Time estimates</t>
+  </si>
+  <si>
+    <t>Expected Time</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Optimistic (O)</t>
+  </si>
+  <si>
+    <t>Normal (M)</t>
+  </si>
+  <si>
+    <t>Pessimistic (P)</t>
+  </si>
+  <si>
+    <t>Concept art for game assets</t>
+  </si>
+  <si>
+    <t>Base Game Framework</t>
+  </si>
+  <si>
+    <t>General Playboard set-up</t>
+  </si>
+  <si>
+    <t>Base Match 3 functions/mechanics</t>
+  </si>
+  <si>
+    <t>Battle Animations</t>
+  </si>
+  <si>
+    <t>Battle Mechanics</t>
+  </si>
+  <si>
+    <t>Adaptive Difficulty</t>
+  </si>
+  <si>
+    <t>Player/Enemy Statistics</t>
+  </si>
+  <si>
+    <t>Predecessor (Refer to ID)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2D Modeling</t>
+  </si>
+  <si>
+    <t>4,8</t>
+  </si>
+  <si>
+    <t>Playboard editor</t>
+  </si>
+  <si>
+    <t>Battle Sequences</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>In-Game Store</t>
+  </si>
+  <si>
+    <t>General In-Game Menu Layout &amp; Design</t>
+  </si>
+  <si>
+    <t>3,5,12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,8 +120,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,8 +168,25 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -97,22 +194,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,52 +569,524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.25" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="5" customWidth="1"/>
+    <col min="2" max="6" width="23.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <f>ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <f t="shared" ref="A4:A15" si="0">ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
+      <c r="B11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="2:6" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>